<commit_message>
updated NIST reference documents spreadsheet
</commit_message>
<xml_diff>
--- a/source/reference_documents/working_material/NIST reference documents.xlsx
+++ b/source/reference_documents/working_material/NIST reference documents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charleswilson/Documents/projects/AVCDL/source/reference_documents/working_material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8BD408-0FBB-3C45-92FD-59174C260896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C9E675-F200-4541-95AB-2462102B2FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21760" yWindow="15660" windowWidth="21640" windowHeight="24480" xr2:uid="{552252AA-65C0-1A41-A97D-6525FC904F70}"/>
+    <workbookView xWindow="52640" yWindow="9700" windowWidth="21640" windowHeight="25660" xr2:uid="{552252AA-65C0-1A41-A97D-6525FC904F70}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
   <si>
     <t>number</t>
   </si>
@@ -279,6 +279,15 @@
   </si>
   <si>
     <t>An Introduction to Information Security</t>
+  </si>
+  <si>
+    <t>Managing Information Security Risk</t>
+  </si>
+  <si>
+    <t>Risk Management Framework for Information Systems and Organizations</t>
+  </si>
+  <si>
+    <t>Mitigating the Risk of Software Vulnerabilities by Adopting a Secure Software Development Framework (SSDF)</t>
   </si>
 </sst>
 </file>
@@ -660,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD588B1-DD28-F24D-9FC3-EB7A429A2AE9}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,74 +738,65 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
-        <v>38</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>37</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
-        <v>41</v>
-      </c>
-      <c r="E6" s="4">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
-        <v>52</v>
-      </c>
-      <c r="E7" s="4">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E8" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
-        <v>57</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="E9" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
-        <v>57</v>
-      </c>
-      <c r="D10" s="4">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="E10" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -804,71 +804,77 @@
         <v>57</v>
       </c>
       <c r="D11" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
-        <v>60</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3</v>
       </c>
       <c r="E13" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
-        <v>63</v>
-      </c>
-      <c r="B14" s="4">
-        <v>3</v>
+        <v>60</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
-        <v>63</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>34</v>
+        <v>61</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>63</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>36</v>
+      <c r="B16" s="4">
+        <v>3</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -876,415 +882,454 @@
         <v>63</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>63</v>
+        <v>34</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
+        <v>63</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="E18" s="4">
-        <v>2</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
-        <v>71</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>21</v>
+        <v>63</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
-        <v>78</v>
-      </c>
-      <c r="B20" s="4">
-        <v>4</v>
+        <v>64</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
-        <v>86</v>
+        <v>71</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
-        <v>88</v>
-      </c>
-      <c r="E22" s="4">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="B22" s="4">
+        <v>4</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
-        <v>102</v>
+        <v>88</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
-        <v>107</v>
-      </c>
-      <c r="E26" s="4">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
-        <v>115</v>
+        <v>107</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
-        <v>125</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="4">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>125</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="G33" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="E34" s="4">
-        <v>3</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>38</v>
+        <v>1</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
-        <v>128</v>
+        <v>125</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
-        <v>131</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="E36" s="4">
-        <v>2</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>40</v>
+        <v>3</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
-        <v>133</v>
-      </c>
-      <c r="E37" s="4">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
-        <v>137</v>
+        <v>131</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="4">
+        <v>2</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
-        <v>140</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>43</v>
+        <v>133</v>
+      </c>
+      <c r="E39" s="4">
+        <v>2</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
-        <v>147</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>45</v>
+        <v>140</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
-        <v>147</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
-        <v>154</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>20</v>
+        <v>147</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
-        <v>160</v>
-      </c>
-      <c r="C45" s="4">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
-        <v>160</v>
-      </c>
-      <c r="C46" s="4">
-        <v>2</v>
+        <v>154</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
-        <v>161</v>
+        <v>160</v>
+      </c>
+      <c r="C47" s="4">
+        <v>1</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
-        <v>171</v>
+        <v>160</v>
+      </c>
+      <c r="C48" s="4">
+        <v>2</v>
       </c>
       <c r="E48" s="4">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
-        <v>175</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>34</v>
+        <v>161</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
-        <v>175</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>36</v>
+        <v>171</v>
       </c>
       <c r="E50" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
-        <v>180</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>20</v>
+        <v>175</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
-        <v>181</v>
+        <v>175</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="E52" s="4">
         <v>1</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="5">
-        <v>184</v>
+        <v>180</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
-        <v>190</v>
+        <v>181</v>
+      </c>
+      <c r="E54" s="4">
+        <v>1</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="5">
+        <v>207</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="5">
+        <v>210</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="5">
         <v>213</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="F61" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G61" s="2" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
+        <v>218</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated NIST references spreadsheet
</commit_message>
<xml_diff>
--- a/source/reference_documents/working_material/NIST reference documents.xlsx
+++ b/source/reference_documents/working_material/NIST reference documents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charleswilson/Documents/projects/AVCDL/source/reference_documents/working_material/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charles.wilson/Documents/projects/AVCDL/source/reference_documents/working_material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C9E675-F200-4541-95AB-2462102B2FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE44F522-102F-BA49-B223-04A256AAD379}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52640" yWindow="9700" windowWidth="21640" windowHeight="25660" xr2:uid="{552252AA-65C0-1A41-A97D-6525FC904F70}"/>
+    <workbookView xWindow="41500" yWindow="5720" windowWidth="21640" windowHeight="25660" xr2:uid="{552252AA-65C0-1A41-A97D-6525FC904F70}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>number</t>
   </si>
@@ -672,7 +672,7 @@
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1175,6 +1175,12 @@
       <c r="C47" s="4">
         <v>1</v>
       </c>
+      <c r="E47" s="4">
+        <v>1</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G47" s="2" t="s">
         <v>53</v>
       </c>

</xml_diff>